<commit_message>
Added legends to corpuses
</commit_message>
<xml_diff>
--- a/corpus/corpus_v1.xlsx
+++ b/corpus/corpus_v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MASTER\TMF\Software-Disambiguation\corpus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9486E17-5EC5-404E-B18F-23AB15FBA747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6B8319-9206-403C-B284-E5F1C2C2545F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Benchmark" sheetId="1" r:id="rId1"/>
@@ -1082,9 +1082,6 @@
     <t>Luca Levrini,L. Paracchini,M. Nosotti</t>
   </si>
   <si>
-    <t>Id of the entry in the benchmark</t>
-  </si>
-  <si>
     <t>mention label as it appears in the original text</t>
   </si>
   <si>
@@ -1785,6 +1782,9 @@
   </si>
   <si>
     <t>https://github.com/scikit-learn/scikit-learn,https://pypi.org/project/scikit-learn/</t>
+  </si>
+  <si>
+    <t>Id of the entry in the corpus</t>
   </si>
 </sst>
 </file>
@@ -2147,7 +2147,7 @@
   </sheetPr>
   <dimension ref="A1:K166"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J133" sqref="J133"/>
     </sheetView>
   </sheetViews>
@@ -2175,7 +2175,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>4</v>
@@ -2196,7 +2196,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2222,13 +2222,13 @@
         <v>15</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2254,13 +2254,13 @@
         <v>21</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2286,13 +2286,13 @@
         <v>26</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2318,13 +2318,13 @@
         <v>31</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2350,13 +2350,13 @@
         <v>36</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2382,13 +2382,13 @@
         <v>42</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K7" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2414,13 +2414,13 @@
         <v>47</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2446,13 +2446,13 @@
         <v>52</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2478,13 +2478,13 @@
         <v>57</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2510,13 +2510,13 @@
         <v>63</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2542,13 +2542,13 @@
         <v>68</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K12" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2574,13 +2574,13 @@
         <v>73</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K13" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2606,13 +2606,13 @@
         <v>79</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K14" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2638,13 +2638,13 @@
         <v>84</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2670,13 +2670,13 @@
         <v>90</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K16" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2702,13 +2702,13 @@
         <v>95</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K17" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2734,13 +2734,13 @@
         <v>100</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K18" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2766,13 +2766,13 @@
         <v>105</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2798,13 +2798,13 @@
         <v>111</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K20" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2830,13 +2830,13 @@
         <v>95</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K21" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2862,13 +2862,13 @@
         <v>95</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K22" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2894,13 +2894,13 @@
         <v>118</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K23" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2926,13 +2926,13 @@
         <v>123</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K24" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2958,13 +2958,13 @@
         <v>123</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K25" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2990,13 +2990,13 @@
         <v>130</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K26" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3022,13 +3022,13 @@
         <v>135</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K27" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3054,13 +3054,13 @@
         <v>26</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K28" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3086,13 +3086,13 @@
         <v>141</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K29" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3118,13 +3118,13 @@
         <v>141</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K30" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3150,13 +3150,13 @@
         <v>147</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K31" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3182,13 +3182,13 @@
         <v>147</v>
       </c>
       <c r="H32" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K32" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3214,13 +3214,13 @@
         <v>147</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I33" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K33" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3246,13 +3246,13 @@
         <v>147</v>
       </c>
       <c r="H34" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K34" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3278,13 +3278,13 @@
         <v>156</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I35" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K35" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3310,13 +3310,13 @@
         <v>161</v>
       </c>
       <c r="H36" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I36" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K36" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3342,13 +3342,13 @@
         <v>166</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I37" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K37" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3374,13 +3374,13 @@
         <v>171</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I38" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K38" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3406,13 +3406,13 @@
         <v>176</v>
       </c>
       <c r="H39" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I39" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K39" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3438,13 +3438,13 @@
         <v>181</v>
       </c>
       <c r="H40" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K40" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3470,13 +3470,13 @@
         <v>187</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I41" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K41" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3502,13 +3502,13 @@
         <v>192</v>
       </c>
       <c r="H42" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I42" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K42" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3534,13 +3534,13 @@
         <v>197</v>
       </c>
       <c r="H43" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K43" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3566,13 +3566,13 @@
         <v>202</v>
       </c>
       <c r="H44" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I44" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K44" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3598,13 +3598,13 @@
         <v>207</v>
       </c>
       <c r="H45" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I45" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K45" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3630,13 +3630,13 @@
         <v>135</v>
       </c>
       <c r="H46" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I46" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K46" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3662,13 +3662,13 @@
         <v>214</v>
       </c>
       <c r="H47" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I47" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K47" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3694,13 +3694,13 @@
         <v>219</v>
       </c>
       <c r="H48" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I48" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K48" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3726,13 +3726,13 @@
         <v>219</v>
       </c>
       <c r="H49" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I49" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K49" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3758,13 +3758,13 @@
         <v>225</v>
       </c>
       <c r="H50" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I50" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K50" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3790,13 +3790,13 @@
         <v>230</v>
       </c>
       <c r="H51" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I51" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K51" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3822,13 +3822,13 @@
         <v>236</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="I52" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K52" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3854,13 +3854,13 @@
         <v>187</v>
       </c>
       <c r="H53" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I53" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K53" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3886,13 +3886,13 @@
         <v>192</v>
       </c>
       <c r="H54" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I54" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K54" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3918,13 +3918,13 @@
         <v>197</v>
       </c>
       <c r="H55" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I55" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K55" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3950,13 +3950,13 @@
         <v>202</v>
       </c>
       <c r="H56" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I56" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K56" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3982,13 +3982,13 @@
         <v>242</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="I57" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K57" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4014,13 +4014,13 @@
         <v>247</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="I58" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K58" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4046,13 +4046,13 @@
         <v>252</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="I59" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K59" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="60" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4078,13 +4078,13 @@
         <v>257</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="I60" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K60" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="61" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4110,13 +4110,13 @@
         <v>262</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="I61" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K61" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="62" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4142,13 +4142,13 @@
         <v>262</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="I62" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K62" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="63" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4174,14 +4174,14 @@
         <v>269</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="I63" s="2" t="s">
         <v>16</v>
       </c>
       <c r="J63" s="2"/>
       <c r="K63" s="4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="64" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4207,13 +4207,13 @@
         <v>274</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="I64" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K64" s="4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="65" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4239,14 +4239,14 @@
         <v>279</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="I65" s="2" t="s">
         <v>16</v>
       </c>
       <c r="J65" s="2"/>
       <c r="K65" s="4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="66" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4272,13 +4272,13 @@
         <v>284</v>
       </c>
       <c r="H66" s="4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="I66" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K66" s="4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="67" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4304,13 +4304,13 @@
         <v>289</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="I67" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K67" s="4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="68" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4336,13 +4336,13 @@
         <v>295</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I68" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K68" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="69" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4368,16 +4368,16 @@
         <v>301</v>
       </c>
       <c r="H69" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="I69" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J69" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="I69" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J69" s="3" t="s">
-        <v>367</v>
-      </c>
       <c r="K69" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="70" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4403,16 +4403,16 @@
         <v>301</v>
       </c>
       <c r="H70" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="I70" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J70" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="I70" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J70" s="3" t="s">
-        <v>367</v>
-      </c>
       <c r="K70" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="71" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4438,16 +4438,16 @@
         <v>301</v>
       </c>
       <c r="H71" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="I71" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J71" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="I71" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J71" s="3" t="s">
-        <v>367</v>
-      </c>
       <c r="K71" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="72" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4473,16 +4473,16 @@
         <v>301</v>
       </c>
       <c r="H72" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J72" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="I72" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J72" s="3" t="s">
-        <v>367</v>
-      </c>
       <c r="K72" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="73" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4508,16 +4508,16 @@
         <v>301</v>
       </c>
       <c r="H73" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="I73" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J73" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="I73" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J73" s="3" t="s">
-        <v>367</v>
-      </c>
       <c r="K73" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="74" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4543,16 +4543,16 @@
         <v>301</v>
       </c>
       <c r="H74" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J74" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="I74" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J74" s="3" t="s">
-        <v>367</v>
-      </c>
       <c r="K74" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="75" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4578,16 +4578,16 @@
         <v>312</v>
       </c>
       <c r="H75" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J75" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="I75" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J75" s="3" t="s">
-        <v>367</v>
-      </c>
       <c r="K75" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="76" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4613,16 +4613,16 @@
         <v>318</v>
       </c>
       <c r="H76" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="I76" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J76" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="I76" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J76" s="3" t="s">
-        <v>367</v>
-      </c>
       <c r="K76" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="77" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4648,16 +4648,16 @@
         <v>321</v>
       </c>
       <c r="H77" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="I77" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J77" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="I77" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J77" s="3" t="s">
-        <v>367</v>
-      </c>
       <c r="K77" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="78" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4683,16 +4683,16 @@
         <v>326</v>
       </c>
       <c r="H78" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="I78" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J78" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="I78" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J78" s="3" t="s">
-        <v>367</v>
-      </c>
       <c r="K78" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="79" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4718,16 +4718,16 @@
         <v>331</v>
       </c>
       <c r="H79" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J79" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="I79" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J79" s="3" t="s">
-        <v>367</v>
-      </c>
       <c r="K79" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="80" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4753,16 +4753,16 @@
         <v>336</v>
       </c>
       <c r="H80" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="I80" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J80" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="I80" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J80" s="3" t="s">
-        <v>367</v>
-      </c>
       <c r="K80" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="81" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4788,16 +4788,16 @@
         <v>342</v>
       </c>
       <c r="H81" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="I81" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J81" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="I81" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J81" s="3" t="s">
-        <v>367</v>
-      </c>
       <c r="K81" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="82" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4823,16 +4823,16 @@
         <v>348</v>
       </c>
       <c r="H82" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="I82" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J82" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="I82" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J82" s="3" t="s">
-        <v>367</v>
-      </c>
       <c r="K82" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="83" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4856,16 +4856,16 @@
       </c>
       <c r="G83" s="2"/>
       <c r="H83" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="I83" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J83" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="I83" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J83" s="3" t="s">
-        <v>367</v>
-      </c>
       <c r="K83" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="84" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4873,34 +4873,34 @@
         <v>83</v>
       </c>
       <c r="B84" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="C84" s="7" t="s">
         <v>368</v>
       </c>
-      <c r="C84" s="7" t="s">
+      <c r="D84" s="7" t="s">
         <v>369</v>
       </c>
-      <c r="D84" s="7" t="s">
+      <c r="E84" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="F84" s="7" t="s">
         <v>370</v>
       </c>
-      <c r="E84" s="7" t="s">
+      <c r="G84" s="7" t="s">
         <v>372</v>
       </c>
-      <c r="F84" s="7" t="s">
-        <v>371</v>
-      </c>
-      <c r="G84" s="7" t="s">
+      <c r="H84" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="I84" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="J84" s="9" t="s">
         <v>373</v>
       </c>
-      <c r="H84" s="8" t="s">
-        <v>375</v>
-      </c>
-      <c r="I84" s="7" t="s">
-        <v>376</v>
-      </c>
-      <c r="J84" s="9" t="s">
+      <c r="K84" s="8" t="s">
         <v>374</v>
-      </c>
-      <c r="K84" s="8" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="85" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4908,34 +4908,34 @@
         <v>84</v>
       </c>
       <c r="B85" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="C85" s="7" t="s">
         <v>377</v>
       </c>
-      <c r="C85" s="7" t="s">
+      <c r="D85" s="7" t="s">
         <v>378</v>
       </c>
-      <c r="D85" s="7" t="s">
+      <c r="E85" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="F85" s="7" t="s">
         <v>379</v>
       </c>
-      <c r="E85" s="7" t="s">
+      <c r="G85" s="7" t="s">
         <v>381</v>
       </c>
-      <c r="F85" s="7" t="s">
-        <v>380</v>
-      </c>
-      <c r="G85" s="7" t="s">
-        <v>382</v>
-      </c>
       <c r="H85" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="I85" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="I85" s="7" t="s">
-        <v>376</v>
-      </c>
       <c r="J85" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="K85" s="8" t="s">
         <v>374</v>
-      </c>
-      <c r="K85" s="8" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="86" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4943,34 +4943,34 @@
         <v>85</v>
       </c>
       <c r="B86" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="C86" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="C86" s="7" t="s">
+      <c r="D86" s="7" t="s">
         <v>384</v>
       </c>
-      <c r="D86" s="7" t="s">
+      <c r="E86" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="F86" s="7" t="s">
         <v>385</v>
       </c>
-      <c r="E86" s="7" t="s">
+      <c r="G86" s="7" t="s">
         <v>387</v>
       </c>
-      <c r="F86" s="7" t="s">
-        <v>386</v>
-      </c>
-      <c r="G86" s="7" t="s">
-        <v>388</v>
-      </c>
       <c r="H86" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="I86" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="I86" s="7" t="s">
-        <v>376</v>
-      </c>
       <c r="J86" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="K86" s="8" t="s">
         <v>374</v>
-      </c>
-      <c r="K86" s="8" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="87" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4978,34 +4978,34 @@
         <v>86</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C87" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="D87" s="7" t="s">
         <v>389</v>
       </c>
-      <c r="D87" s="7" t="s">
+      <c r="E87" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="F87" s="7" t="s">
         <v>390</v>
       </c>
-      <c r="E87" s="7" t="s">
+      <c r="G87" s="7" t="s">
         <v>392</v>
       </c>
-      <c r="F87" s="7" t="s">
-        <v>391</v>
-      </c>
-      <c r="G87" s="7" t="s">
-        <v>393</v>
-      </c>
       <c r="H87" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="I87" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="I87" s="7" t="s">
-        <v>376</v>
-      </c>
       <c r="J87" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="K87" s="8" t="s">
         <v>374</v>
-      </c>
-      <c r="K87" s="8" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="88" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5013,34 +5013,34 @@
         <v>87</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C88" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="D88" s="7" t="s">
         <v>394</v>
       </c>
-      <c r="D88" s="7" t="s">
+      <c r="E88" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="F88" s="7" t="s">
         <v>395</v>
       </c>
-      <c r="E88" s="7" t="s">
+      <c r="G88" s="7" t="s">
         <v>397</v>
       </c>
-      <c r="F88" s="7" t="s">
-        <v>396</v>
-      </c>
-      <c r="G88" s="7" t="s">
-        <v>398</v>
-      </c>
       <c r="H88" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="I88" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="I88" s="7" t="s">
-        <v>376</v>
-      </c>
       <c r="J88" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="K88" s="8" t="s">
         <v>374</v>
-      </c>
-      <c r="K88" s="8" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="89" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5048,34 +5048,34 @@
         <v>88</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C89" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="D89" s="7" t="s">
         <v>399</v>
       </c>
-      <c r="D89" s="7" t="s">
+      <c r="E89" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="F89" s="7" t="s">
         <v>400</v>
       </c>
-      <c r="E89" s="7" t="s">
+      <c r="G89" s="7" t="s">
         <v>402</v>
       </c>
-      <c r="F89" s="7" t="s">
-        <v>401</v>
-      </c>
-      <c r="G89" s="7" t="s">
-        <v>403</v>
-      </c>
       <c r="H89" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="I89" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="I89" s="7" t="s">
-        <v>376</v>
-      </c>
       <c r="J89" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="K89" s="8" t="s">
         <v>374</v>
-      </c>
-      <c r="K89" s="8" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="90" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5083,34 +5083,34 @@
         <v>89</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C90" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="D90" s="7" t="s">
         <v>404</v>
       </c>
-      <c r="D90" s="7" t="s">
+      <c r="E90" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="F90" s="7" t="s">
         <v>405</v>
       </c>
-      <c r="E90" s="7" t="s">
+      <c r="G90" s="7" t="s">
         <v>407</v>
       </c>
-      <c r="F90" s="7" t="s">
-        <v>406</v>
-      </c>
-      <c r="G90" s="7" t="s">
-        <v>408</v>
-      </c>
       <c r="H90" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="I90" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="I90" s="7" t="s">
-        <v>376</v>
-      </c>
       <c r="J90" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="K90" s="8" t="s">
         <v>374</v>
-      </c>
-      <c r="K90" s="8" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="91" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5118,34 +5118,34 @@
         <v>90</v>
       </c>
       <c r="B91" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="C91" s="7" t="s">
         <v>409</v>
       </c>
-      <c r="C91" s="7" t="s">
+      <c r="D91" s="7" t="s">
         <v>410</v>
       </c>
-      <c r="D91" s="7" t="s">
+      <c r="E91" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="F91" s="7" t="s">
         <v>411</v>
       </c>
-      <c r="E91" s="7" t="s">
+      <c r="G91" s="7" t="s">
         <v>413</v>
       </c>
-      <c r="F91" s="7" t="s">
-        <v>412</v>
-      </c>
-      <c r="G91" s="7" t="s">
-        <v>414</v>
-      </c>
       <c r="H91" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="I91" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="I91" s="7" t="s">
-        <v>376</v>
-      </c>
       <c r="J91" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="K91" s="8" t="s">
         <v>374</v>
-      </c>
-      <c r="K91" s="8" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="92" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5153,34 +5153,34 @@
         <v>91</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C92" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="D92" s="7" t="s">
         <v>415</v>
       </c>
-      <c r="D92" s="7" t="s">
+      <c r="E92" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="F92" s="7" t="s">
         <v>416</v>
       </c>
-      <c r="E92" s="7" t="s">
+      <c r="G92" s="7" t="s">
         <v>418</v>
       </c>
-      <c r="F92" s="7" t="s">
-        <v>417</v>
-      </c>
-      <c r="G92" s="7" t="s">
-        <v>419</v>
-      </c>
       <c r="H92" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="I92" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="I92" s="7" t="s">
-        <v>376</v>
-      </c>
       <c r="J92" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="K92" s="8" t="s">
         <v>374</v>
-      </c>
-      <c r="K92" s="8" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="93" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5188,34 +5188,34 @@
         <v>92</v>
       </c>
       <c r="B93" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="C93" s="7" t="s">
         <v>420</v>
       </c>
-      <c r="C93" s="7" t="s">
+      <c r="D93" s="7" t="s">
         <v>421</v>
       </c>
-      <c r="D93" s="7" t="s">
+      <c r="E93" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="F93" s="7" t="s">
         <v>422</v>
       </c>
-      <c r="E93" s="7" t="s">
+      <c r="G93" s="7" t="s">
         <v>424</v>
       </c>
-      <c r="F93" s="7" t="s">
-        <v>423</v>
-      </c>
-      <c r="G93" s="7" t="s">
-        <v>425</v>
-      </c>
       <c r="H93" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="I93" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="I93" s="7" t="s">
-        <v>376</v>
-      </c>
       <c r="J93" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="K93" s="8" t="s">
         <v>374</v>
-      </c>
-      <c r="K93" s="8" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="94" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5223,34 +5223,34 @@
         <v>93</v>
       </c>
       <c r="B94" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="C94" s="7" t="s">
         <v>420</v>
       </c>
-      <c r="C94" s="7" t="s">
-        <v>421</v>
-      </c>
       <c r="D94" s="7" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E94" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="F94" s="7" t="s">
+        <v>422</v>
+      </c>
+      <c r="G94" s="7" t="s">
         <v>424</v>
       </c>
-      <c r="F94" s="7" t="s">
-        <v>423</v>
-      </c>
-      <c r="G94" s="7" t="s">
-        <v>425</v>
-      </c>
       <c r="H94" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="I94" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="I94" s="7" t="s">
-        <v>376</v>
-      </c>
       <c r="J94" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="K94" s="8" t="s">
         <v>374</v>
-      </c>
-      <c r="K94" s="8" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="95" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5258,34 +5258,34 @@
         <v>94</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C95" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="D95" s="7" t="s">
         <v>427</v>
       </c>
-      <c r="D95" s="7" t="s">
+      <c r="E95" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="F95" s="7" t="s">
         <v>428</v>
       </c>
-      <c r="E95" s="7" t="s">
+      <c r="G95" s="7" t="s">
         <v>430</v>
       </c>
-      <c r="F95" s="7" t="s">
-        <v>429</v>
-      </c>
-      <c r="G95" s="7" t="s">
-        <v>431</v>
-      </c>
       <c r="H95" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="I95" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="I95" s="7" t="s">
-        <v>376</v>
-      </c>
       <c r="J95" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="K95" s="8" t="s">
         <v>374</v>
-      </c>
-      <c r="K95" s="8" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="96" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5293,34 +5293,34 @@
         <v>95</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C96" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="D96" s="7" t="s">
         <v>432</v>
       </c>
-      <c r="D96" s="7" t="s">
+      <c r="E96" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="F96" s="7" t="s">
         <v>433</v>
       </c>
-      <c r="E96" s="7" t="s">
+      <c r="G96" s="7" t="s">
         <v>435</v>
       </c>
-      <c r="F96" s="7" t="s">
-        <v>434</v>
-      </c>
-      <c r="G96" s="7" t="s">
-        <v>436</v>
-      </c>
       <c r="H96" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="I96" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="I96" s="7" t="s">
-        <v>376</v>
-      </c>
       <c r="J96" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="K96" s="8" t="s">
         <v>374</v>
-      </c>
-      <c r="K96" s="8" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="97" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5328,34 +5328,34 @@
         <v>96</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C97" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="D97" s="7" t="s">
         <v>437</v>
       </c>
-      <c r="D97" s="7" t="s">
+      <c r="E97" s="7" t="s">
+        <v>439</v>
+      </c>
+      <c r="F97" s="7" t="s">
         <v>438</v>
       </c>
-      <c r="E97" s="7" t="s">
+      <c r="G97" s="7" t="s">
         <v>440</v>
       </c>
-      <c r="F97" s="7" t="s">
-        <v>439</v>
-      </c>
-      <c r="G97" s="7" t="s">
-        <v>441</v>
-      </c>
       <c r="H97" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="I97" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="I97" s="7" t="s">
-        <v>376</v>
-      </c>
       <c r="J97" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="K97" s="8" t="s">
         <v>374</v>
-      </c>
-      <c r="K97" s="8" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="98" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5363,34 +5363,34 @@
         <v>97</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C98" s="7" t="s">
+        <v>441</v>
+      </c>
+      <c r="D98" s="7" t="s">
         <v>442</v>
       </c>
-      <c r="D98" s="7" t="s">
+      <c r="E98" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="F98" s="7" t="s">
         <v>443</v>
       </c>
-      <c r="E98" s="7" t="s">
+      <c r="G98" s="7" t="s">
         <v>445</v>
       </c>
-      <c r="F98" s="7" t="s">
-        <v>444</v>
-      </c>
-      <c r="G98" s="7" t="s">
-        <v>446</v>
-      </c>
       <c r="H98" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="I98" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="I98" s="7" t="s">
-        <v>376</v>
-      </c>
       <c r="J98" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="K98" s="8" t="s">
         <v>374</v>
-      </c>
-      <c r="K98" s="8" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="99" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5398,34 +5398,34 @@
         <v>98</v>
       </c>
       <c r="B99" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="C99" s="7" t="s">
         <v>447</v>
       </c>
-      <c r="C99" s="7" t="s">
+      <c r="D99" s="7" t="s">
         <v>448</v>
       </c>
-      <c r="D99" s="7" t="s">
+      <c r="E99" s="7" t="s">
+        <v>450</v>
+      </c>
+      <c r="F99" s="7" t="s">
         <v>449</v>
       </c>
-      <c r="E99" s="7" t="s">
+      <c r="G99" s="7" t="s">
         <v>451</v>
       </c>
-      <c r="F99" s="7" t="s">
-        <v>450</v>
-      </c>
-      <c r="G99" s="7" t="s">
-        <v>452</v>
-      </c>
       <c r="H99" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="I99" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="I99" s="7" t="s">
-        <v>376</v>
-      </c>
       <c r="J99" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="K99" s="8" t="s">
         <v>374</v>
-      </c>
-      <c r="K99" s="8" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="100" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5433,34 +5433,34 @@
         <v>99</v>
       </c>
       <c r="B100" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="C100" s="7" t="s">
         <v>453</v>
       </c>
-      <c r="C100" s="7" t="s">
+      <c r="D100" s="7" t="s">
         <v>454</v>
       </c>
-      <c r="D100" s="7" t="s">
+      <c r="E100" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="F100" s="7" t="s">
         <v>455</v>
       </c>
-      <c r="E100" s="7" t="s">
+      <c r="G100" s="7" t="s">
         <v>457</v>
       </c>
-      <c r="F100" s="7" t="s">
-        <v>456</v>
-      </c>
-      <c r="G100" s="7" t="s">
+      <c r="H100" s="8" t="s">
         <v>458</v>
       </c>
-      <c r="H100" s="8" t="s">
-        <v>459</v>
-      </c>
       <c r="I100" s="7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J100" s="9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="K100" s="8" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="101" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5468,34 +5468,34 @@
         <v>100</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C101" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="D101" s="7" t="s">
         <v>460</v>
       </c>
-      <c r="D101" s="7" t="s">
+      <c r="E101" s="7" t="s">
+        <v>462</v>
+      </c>
+      <c r="F101" s="7" t="s">
         <v>461</v>
       </c>
-      <c r="E101" s="7" t="s">
+      <c r="G101" s="7" t="s">
         <v>463</v>
       </c>
-      <c r="F101" s="7" t="s">
-        <v>462</v>
-      </c>
-      <c r="G101" s="7" t="s">
-        <v>464</v>
-      </c>
       <c r="H101" s="8" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="I101" s="7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J101" s="9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="K101" s="8" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="102" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5503,34 +5503,34 @@
         <v>101</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C102" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="D102" s="7" t="s">
         <v>465</v>
       </c>
-      <c r="D102" s="7" t="s">
+      <c r="E102" s="7" t="s">
+        <v>467</v>
+      </c>
+      <c r="F102" s="7" t="s">
         <v>466</v>
       </c>
-      <c r="E102" s="7" t="s">
+      <c r="G102" s="7" t="s">
         <v>468</v>
       </c>
-      <c r="F102" s="7" t="s">
-        <v>467</v>
-      </c>
-      <c r="G102" s="7" t="s">
-        <v>469</v>
-      </c>
       <c r="H102" s="8" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="I102" s="7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J102" s="9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="K102" s="8" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="103" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5538,34 +5538,34 @@
         <v>102</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C103" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="D103" s="7" t="s">
         <v>470</v>
       </c>
-      <c r="D103" s="7" t="s">
+      <c r="E103" s="7" t="s">
+        <v>472</v>
+      </c>
+      <c r="F103" s="7" t="s">
         <v>471</v>
       </c>
-      <c r="E103" s="7" t="s">
+      <c r="G103" s="7" t="s">
         <v>473</v>
       </c>
-      <c r="F103" s="7" t="s">
-        <v>472</v>
-      </c>
-      <c r="G103" s="7" t="s">
-        <v>474</v>
-      </c>
       <c r="H103" s="8" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="I103" s="7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J103" s="9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="K103" s="8" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="104" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5573,34 +5573,34 @@
         <v>103</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C104" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="D104" s="7" t="s">
         <v>475</v>
       </c>
-      <c r="D104" s="7" t="s">
+      <c r="E104" s="7" t="s">
+        <v>477</v>
+      </c>
+      <c r="F104" s="7" t="s">
         <v>476</v>
       </c>
-      <c r="E104" s="7" t="s">
+      <c r="G104" s="7" t="s">
         <v>478</v>
       </c>
-      <c r="F104" s="7" t="s">
-        <v>477</v>
-      </c>
-      <c r="G104" s="7" t="s">
-        <v>479</v>
-      </c>
       <c r="H104" s="8" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="I104" s="7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J104" s="9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="K104" s="8" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="105" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5608,34 +5608,34 @@
         <v>104</v>
       </c>
       <c r="B105" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="C105" s="7" t="s">
         <v>480</v>
       </c>
-      <c r="C105" s="7" t="s">
+      <c r="D105" s="7" t="s">
         <v>481</v>
       </c>
-      <c r="D105" s="7" t="s">
+      <c r="E105" s="7" t="s">
+        <v>483</v>
+      </c>
+      <c r="F105" s="7" t="s">
         <v>482</v>
       </c>
-      <c r="E105" s="7" t="s">
+      <c r="G105" s="7" t="s">
         <v>484</v>
       </c>
-      <c r="F105" s="7" t="s">
-        <v>483</v>
-      </c>
-      <c r="G105" s="7" t="s">
-        <v>485</v>
-      </c>
       <c r="H105" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="I105" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="I105" s="7" t="s">
-        <v>376</v>
-      </c>
       <c r="J105" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="K105" s="8" t="s">
         <v>374</v>
-      </c>
-      <c r="K105" s="8" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="106" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5643,34 +5643,34 @@
         <v>105</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C106" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="D106" s="7" t="s">
         <v>486</v>
       </c>
-      <c r="D106" s="7" t="s">
+      <c r="E106" s="7" t="s">
+        <v>488</v>
+      </c>
+      <c r="F106" s="7" t="s">
         <v>487</v>
       </c>
-      <c r="E106" s="7" t="s">
+      <c r="G106" s="7" t="s">
         <v>489</v>
       </c>
-      <c r="F106" s="7" t="s">
-        <v>488</v>
-      </c>
-      <c r="G106" s="7" t="s">
-        <v>490</v>
-      </c>
       <c r="H106" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="I106" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="I106" s="7" t="s">
-        <v>376</v>
-      </c>
       <c r="J106" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="K106" s="10" t="s">
         <v>374</v>
-      </c>
-      <c r="K106" s="10" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="107" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5678,34 +5678,34 @@
         <v>106</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C107" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="D107" s="7" t="s">
         <v>491</v>
       </c>
-      <c r="D107" s="7" t="s">
+      <c r="E107" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="F107" s="7" t="s">
         <v>492</v>
       </c>
-      <c r="E107" s="7" t="s">
+      <c r="G107" s="7" t="s">
         <v>494</v>
       </c>
-      <c r="F107" s="7" t="s">
-        <v>493</v>
-      </c>
-      <c r="G107" s="7" t="s">
-        <v>495</v>
-      </c>
       <c r="H107" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="I107" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="I107" s="7" t="s">
-        <v>376</v>
-      </c>
       <c r="J107" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="K107" s="10" t="s">
         <v>374</v>
-      </c>
-      <c r="K107" s="10" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="108" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5713,34 +5713,34 @@
         <v>107</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C108" s="7" t="s">
+        <v>495</v>
+      </c>
+      <c r="D108" s="7" t="s">
         <v>496</v>
       </c>
-      <c r="D108" s="7" t="s">
+      <c r="E108" s="7" t="s">
+        <v>498</v>
+      </c>
+      <c r="F108" s="7" t="s">
         <v>497</v>
       </c>
-      <c r="E108" s="7" t="s">
+      <c r="G108" s="7" t="s">
         <v>499</v>
       </c>
-      <c r="F108" s="7" t="s">
-        <v>498</v>
-      </c>
-      <c r="G108" s="7" t="s">
-        <v>500</v>
-      </c>
       <c r="H108" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="I108" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="I108" s="7" t="s">
-        <v>376</v>
-      </c>
       <c r="J108" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="K108" s="10" t="s">
         <v>374</v>
-      </c>
-      <c r="K108" s="10" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="109" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5748,34 +5748,34 @@
         <v>108</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C109" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="D109" s="7" t="s">
         <v>501</v>
       </c>
-      <c r="D109" s="7" t="s">
+      <c r="E109" s="7" t="s">
+        <v>503</v>
+      </c>
+      <c r="F109" s="7" t="s">
         <v>502</v>
       </c>
-      <c r="E109" s="7" t="s">
+      <c r="G109" s="7" t="s">
         <v>504</v>
       </c>
-      <c r="F109" s="7" t="s">
-        <v>503</v>
-      </c>
-      <c r="G109" s="7" t="s">
-        <v>505</v>
-      </c>
       <c r="H109" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="I109" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="I109" s="7" t="s">
-        <v>376</v>
-      </c>
       <c r="J109" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="K109" s="10" t="s">
         <v>374</v>
-      </c>
-      <c r="K109" s="10" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="110" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5783,34 +5783,34 @@
         <v>109</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C110" s="7" t="s">
+        <v>505</v>
+      </c>
+      <c r="D110" s="7" t="s">
         <v>506</v>
       </c>
-      <c r="D110" s="7" t="s">
+      <c r="E110" s="7" t="s">
+        <v>508</v>
+      </c>
+      <c r="F110" s="7" t="s">
         <v>507</v>
       </c>
-      <c r="E110" s="7" t="s">
+      <c r="G110" s="7" t="s">
         <v>509</v>
       </c>
-      <c r="F110" s="7" t="s">
-        <v>508</v>
-      </c>
-      <c r="G110" s="7" t="s">
-        <v>510</v>
-      </c>
       <c r="H110" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="I110" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="I110" s="7" t="s">
-        <v>376</v>
-      </c>
       <c r="J110" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="K110" s="10" t="s">
         <v>374</v>
-      </c>
-      <c r="K110" s="10" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="111" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5818,34 +5818,34 @@
         <v>110</v>
       </c>
       <c r="B111" s="6" t="s">
+        <v>510</v>
+      </c>
+      <c r="C111" s="7" t="s">
         <v>511</v>
       </c>
-      <c r="C111" s="7" t="s">
+      <c r="D111" s="7" t="s">
         <v>512</v>
       </c>
-      <c r="D111" s="7" t="s">
+      <c r="E111" s="7" t="s">
+        <v>514</v>
+      </c>
+      <c r="F111" s="7" t="s">
         <v>513</v>
       </c>
-      <c r="E111" s="7" t="s">
+      <c r="G111" s="7" t="s">
         <v>515</v>
       </c>
-      <c r="F111" s="7" t="s">
-        <v>514</v>
-      </c>
-      <c r="G111" s="7" t="s">
-        <v>516</v>
-      </c>
       <c r="H111" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="I111" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="I111" s="7" t="s">
-        <v>376</v>
-      </c>
       <c r="J111" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="K111" s="10" t="s">
         <v>374</v>
-      </c>
-      <c r="K111" s="10" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="112" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5853,34 +5853,34 @@
         <v>111</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C112" s="7" t="s">
+        <v>516</v>
+      </c>
+      <c r="D112" s="7" t="s">
         <v>517</v>
       </c>
-      <c r="D112" s="7" t="s">
+      <c r="E112" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="F112" s="7" t="s">
         <v>518</v>
       </c>
-      <c r="E112" s="7" t="s">
+      <c r="G112" s="7" t="s">
         <v>520</v>
       </c>
-      <c r="F112" s="7" t="s">
-        <v>519</v>
-      </c>
-      <c r="G112" s="7" t="s">
-        <v>521</v>
-      </c>
       <c r="H112" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="I112" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="I112" s="7" t="s">
-        <v>376</v>
-      </c>
       <c r="J112" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="K112" s="10" t="s">
         <v>374</v>
-      </c>
-      <c r="K112" s="10" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="113" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5888,34 +5888,34 @@
         <v>112</v>
       </c>
       <c r="B113" s="6" t="s">
+        <v>521</v>
+      </c>
+      <c r="C113" s="7" t="s">
         <v>522</v>
       </c>
-      <c r="C113" s="7" t="s">
+      <c r="D113" s="7" t="s">
         <v>523</v>
       </c>
-      <c r="D113" s="7" t="s">
+      <c r="E113" s="7" t="s">
+        <v>525</v>
+      </c>
+      <c r="F113" s="7" t="s">
         <v>524</v>
       </c>
-      <c r="E113" s="7" t="s">
+      <c r="G113" s="7" t="s">
         <v>526</v>
       </c>
-      <c r="F113" s="7" t="s">
-        <v>525</v>
-      </c>
-      <c r="G113" s="7" t="s">
-        <v>527</v>
-      </c>
       <c r="H113" s="12" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="I113" s="7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J113" s="9" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="K113" s="12" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="114" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5923,34 +5923,34 @@
         <v>113</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C114" s="7" t="s">
+        <v>527</v>
+      </c>
+      <c r="D114" s="7" t="s">
         <v>528</v>
       </c>
-      <c r="D114" s="7" t="s">
+      <c r="E114" s="7" t="s">
+        <v>530</v>
+      </c>
+      <c r="F114" s="7" t="s">
         <v>529</v>
       </c>
-      <c r="E114" s="7" t="s">
+      <c r="G114" s="7" t="s">
         <v>531</v>
       </c>
-      <c r="F114" s="7" t="s">
-        <v>530</v>
-      </c>
-      <c r="G114" s="7" t="s">
-        <v>532</v>
-      </c>
       <c r="H114" s="12" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="I114" s="7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J114" s="9" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="K114" s="12" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="115" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5958,34 +5958,34 @@
         <v>114</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C115" s="7" t="s">
+        <v>532</v>
+      </c>
+      <c r="D115" s="7" t="s">
         <v>533</v>
       </c>
-      <c r="D115" s="7" t="s">
+      <c r="E115" s="7" t="s">
+        <v>535</v>
+      </c>
+      <c r="F115" s="7" t="s">
         <v>534</v>
       </c>
-      <c r="E115" s="7" t="s">
+      <c r="G115" s="7" t="s">
         <v>536</v>
       </c>
-      <c r="F115" s="7" t="s">
-        <v>535</v>
-      </c>
-      <c r="G115" s="7" t="s">
-        <v>537</v>
-      </c>
       <c r="H115" s="12" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="I115" s="7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J115" s="9" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="K115" s="12" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="116" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5993,34 +5993,34 @@
         <v>115</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C116" s="7" t="s">
+        <v>537</v>
+      </c>
+      <c r="D116" s="7" t="s">
         <v>538</v>
       </c>
-      <c r="D116" s="7" t="s">
+      <c r="E116" s="7" t="s">
+        <v>540</v>
+      </c>
+      <c r="F116" s="7" t="s">
         <v>539</v>
       </c>
-      <c r="E116" s="7" t="s">
+      <c r="G116" s="7" t="s">
         <v>541</v>
       </c>
-      <c r="F116" s="7" t="s">
-        <v>540</v>
-      </c>
-      <c r="G116" s="7" t="s">
-        <v>542</v>
-      </c>
       <c r="H116" s="12" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="I116" s="7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J116" s="9" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="K116" s="12" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="117" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6028,34 +6028,34 @@
         <v>116</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C117" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="D117" s="7" t="s">
         <v>543</v>
       </c>
-      <c r="D117" s="7" t="s">
+      <c r="E117" s="7" t="s">
+        <v>545</v>
+      </c>
+      <c r="F117" s="7" t="s">
         <v>544</v>
       </c>
-      <c r="E117" s="7" t="s">
+      <c r="G117" s="7" t="s">
         <v>546</v>
       </c>
-      <c r="F117" s="7" t="s">
-        <v>545</v>
-      </c>
-      <c r="G117" s="7" t="s">
-        <v>547</v>
-      </c>
       <c r="H117" s="12" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="I117" s="7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J117" s="9" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="K117" s="12" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="118" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6063,34 +6063,34 @@
         <v>117</v>
       </c>
       <c r="B118" s="6" t="s">
+        <v>547</v>
+      </c>
+      <c r="C118" s="7" t="s">
         <v>548</v>
       </c>
-      <c r="C118" s="7" t="s">
+      <c r="D118" s="7" t="s">
         <v>549</v>
       </c>
-      <c r="D118" s="7" t="s">
+      <c r="E118" s="7" t="s">
+        <v>551</v>
+      </c>
+      <c r="F118" s="7" t="s">
         <v>550</v>
       </c>
-      <c r="E118" s="7" t="s">
+      <c r="G118" s="7" t="s">
         <v>552</v>
       </c>
-      <c r="F118" s="7" t="s">
-        <v>551</v>
-      </c>
-      <c r="G118" s="7" t="s">
-        <v>553</v>
-      </c>
       <c r="H118" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="I118" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="I118" s="7" t="s">
-        <v>376</v>
-      </c>
       <c r="J118" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="K118" s="8" t="s">
         <v>374</v>
-      </c>
-      <c r="K118" s="8" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="119" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6098,34 +6098,34 @@
         <v>118</v>
       </c>
       <c r="B119" s="6" t="s">
+        <v>553</v>
+      </c>
+      <c r="C119" s="7" t="s">
         <v>554</v>
       </c>
-      <c r="C119" s="7" t="s">
+      <c r="D119" s="7" t="s">
         <v>555</v>
       </c>
-      <c r="D119" s="7" t="s">
+      <c r="E119" s="7" t="s">
+        <v>557</v>
+      </c>
+      <c r="F119" s="7" t="s">
         <v>556</v>
       </c>
-      <c r="E119" s="7" t="s">
+      <c r="G119" s="7" t="s">
         <v>558</v>
       </c>
-      <c r="F119" s="7" t="s">
-        <v>557</v>
-      </c>
-      <c r="G119" s="7" t="s">
-        <v>559</v>
-      </c>
       <c r="H119" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="I119" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="I119" s="7" t="s">
-        <v>376</v>
-      </c>
       <c r="J119" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="K119" s="8" t="s">
         <v>374</v>
-      </c>
-      <c r="K119" s="8" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="120" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6133,34 +6133,34 @@
         <v>119</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C120" s="7" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D120" s="7" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="E120" s="7" t="s">
+        <v>551</v>
+      </c>
+      <c r="F120" s="7" t="s">
+        <v>550</v>
+      </c>
+      <c r="G120" s="7" t="s">
         <v>552</v>
       </c>
-      <c r="F120" s="7" t="s">
-        <v>551</v>
-      </c>
-      <c r="G120" s="7" t="s">
-        <v>553</v>
-      </c>
       <c r="H120" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="I120" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="I120" s="7" t="s">
-        <v>376</v>
-      </c>
       <c r="J120" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="K120" s="8" t="s">
         <v>374</v>
-      </c>
-      <c r="K120" s="8" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="121" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6168,34 +6168,34 @@
         <v>120</v>
       </c>
       <c r="B121" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="C121" s="7" t="s">
         <v>561</v>
       </c>
-      <c r="C121" s="7" t="s">
+      <c r="D121" s="7" t="s">
         <v>562</v>
       </c>
-      <c r="D121" s="7" t="s">
+      <c r="E121" s="7" t="s">
+        <v>564</v>
+      </c>
+      <c r="F121" s="7" t="s">
         <v>563</v>
       </c>
-      <c r="E121" s="7" t="s">
+      <c r="G121" s="7" t="s">
         <v>565</v>
       </c>
-      <c r="F121" s="7" t="s">
-        <v>564</v>
-      </c>
-      <c r="G121" s="7" t="s">
-        <v>566</v>
-      </c>
       <c r="H121" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="I121" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="I121" s="7" t="s">
-        <v>376</v>
-      </c>
       <c r="J121" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="K121" s="8" t="s">
         <v>374</v>
-      </c>
-      <c r="K121" s="8" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="122" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6203,34 +6203,34 @@
         <v>121</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C122" s="7" t="s">
+        <v>566</v>
+      </c>
+      <c r="D122" s="7" t="s">
         <v>567</v>
       </c>
-      <c r="D122" s="7" t="s">
+      <c r="E122" s="7" t="s">
+        <v>569</v>
+      </c>
+      <c r="F122" s="7" t="s">
         <v>568</v>
       </c>
-      <c r="E122" s="7" t="s">
+      <c r="G122" s="7" t="s">
         <v>570</v>
       </c>
-      <c r="F122" s="7" t="s">
-        <v>569</v>
-      </c>
-      <c r="G122" s="7" t="s">
-        <v>571</v>
-      </c>
       <c r="H122" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="I122" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="I122" s="7" t="s">
-        <v>376</v>
-      </c>
       <c r="J122" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="K122" s="8" t="s">
         <v>374</v>
-      </c>
-      <c r="K122" s="8" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="123" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6238,34 +6238,34 @@
         <v>122</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C123" s="7" t="s">
+        <v>571</v>
+      </c>
+      <c r="D123" s="7" t="s">
         <v>572</v>
       </c>
-      <c r="D123" s="7" t="s">
+      <c r="E123" s="7" t="s">
+        <v>574</v>
+      </c>
+      <c r="F123" s="7" t="s">
         <v>573</v>
       </c>
-      <c r="E123" s="7" t="s">
+      <c r="G123" s="7" t="s">
         <v>575</v>
       </c>
-      <c r="F123" s="7" t="s">
-        <v>574</v>
-      </c>
-      <c r="G123" s="7" t="s">
-        <v>576</v>
-      </c>
       <c r="H123" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="I123" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="I123" s="7" t="s">
-        <v>376</v>
-      </c>
       <c r="J123" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="K123" s="8" t="s">
         <v>374</v>
-      </c>
-      <c r="K123" s="8" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="124" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6273,34 +6273,34 @@
         <v>123</v>
       </c>
       <c r="B124" s="6" t="s">
+        <v>576</v>
+      </c>
+      <c r="C124" s="7" t="s">
         <v>577</v>
       </c>
-      <c r="C124" s="7" t="s">
+      <c r="D124" s="7" t="s">
         <v>578</v>
       </c>
-      <c r="D124" s="7" t="s">
+      <c r="E124" s="11" t="s">
+        <v>580</v>
+      </c>
+      <c r="F124" s="7" t="s">
         <v>579</v>
       </c>
-      <c r="E124" s="11" t="s">
+      <c r="G124" s="7" t="s">
         <v>581</v>
       </c>
-      <c r="F124" s="7" t="s">
-        <v>580</v>
-      </c>
-      <c r="G124" s="7" t="s">
-        <v>582</v>
-      </c>
       <c r="H124" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="I124" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="I124" s="7" t="s">
-        <v>376</v>
-      </c>
       <c r="J124" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="K124" s="8" t="s">
         <v>374</v>
-      </c>
-      <c r="K124" s="8" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="126" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6581,8 +6581,8 @@
   </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6592,7 +6592,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>353</v>
+        <v>587</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -6600,7 +6600,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -6608,7 +6608,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -6616,7 +6616,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -6624,7 +6624,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -6632,7 +6632,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -6640,15 +6640,15 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>360</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -6656,7 +6656,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>

</xml_diff>